<commit_message>
New Stuff (categorial CDE ethnicity)
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-cde-sex-assigned-at-birth.xlsx
+++ b/output/StructureDefinition-cde-sex-assigned-at-birth.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-03-03T12:59:12+01:00</t>
+    <t>2023-03-03T15:59:45+01:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -84,7 +84,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Dieses CDE enthält das 'bei Geburt zugewiesene Geschlecht' einer Person.</t>
+    <t>Dieses CDE enthält das 'bei Geburt zugewiesene Geschlecht'.</t>
   </si>
   <si>
     <t>Purpose</t>

</xml_diff>

<commit_message>
Update (Slicing Fehler in CDE_SexAssignedAtBirth behoben)
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-cde-sex-assigned-at-birth.xlsx
+++ b/output/StructureDefinition-cde-sex-assigned-at-birth.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5196" uniqueCount="623">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5195" uniqueCount="624">
   <si>
     <t>Property</t>
   </si>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-03-04T03:06:34+01:00</t>
+    <t>2023-03-04T04:05:22+01:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1399,10 +1399,6 @@
     <t>Observation.value[x]</t>
   </si>
   <si>
-    <t>Quantity
-CodeableConceptstringbooleanintegerRangeRatioSampledDatatimedateTimePeriod</t>
-  </si>
-  <si>
     <t>Actual result</t>
   </si>
   <si>
@@ -1413,6 +1409,10 @@
   </si>
   <si>
     <t>An observation exists to have a value, though it might not if it is in error, or if it represents a group of observations.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">type:$this}
+</t>
   </si>
   <si>
     <t>ele-1
@@ -1916,6 +1916,10 @@
   </si>
   <si>
     <t>Observation.component.value[x]</t>
+  </si>
+  <si>
+    <t>Quantity
+CodeableConceptstringbooleanintegerRangeRatioSampledDatatimedateTimePeriod</t>
   </si>
   <si>
     <t>Actual component result</t>
@@ -15038,13 +15042,13 @@
       </c>
       <c r="E106" s="2"/>
       <c r="F106" t="s" s="2">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="G106" t="s" s="2">
         <v>92</v>
       </c>
       <c r="H106" t="s" s="2">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="I106" t="s" s="2">
         <v>82</v>
@@ -15053,19 +15057,19 @@
         <v>93</v>
       </c>
       <c r="K106" t="s" s="2">
+        <v>198</v>
+      </c>
+      <c r="L106" t="s" s="2">
         <v>448</v>
       </c>
-      <c r="L106" t="s" s="2">
+      <c r="M106" t="s" s="2">
         <v>449</v>
       </c>
-      <c r="M106" t="s" s="2">
+      <c r="N106" t="s" s="2">
         <v>450</v>
       </c>
-      <c r="N106" t="s" s="2">
+      <c r="O106" t="s" s="2">
         <v>451</v>
-      </c>
-      <c r="O106" t="s" s="2">
-        <v>452</v>
       </c>
       <c r="P106" t="s" s="2">
         <v>82</v>
@@ -15102,16 +15106,14 @@
         <v>82</v>
       </c>
       <c r="AB106" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AC106" t="s" s="2">
-        <v>82</v>
-      </c>
+        <v>452</v>
+      </c>
+      <c r="AC106" s="2"/>
       <c r="AD106" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AE106" t="s" s="2">
-        <v>82</v>
+        <v>146</v>
       </c>
       <c r="AF106" t="s" s="2">
         <v>447</v>
@@ -18075,19 +18077,19 @@
         <v>93</v>
       </c>
       <c r="K131" t="s" s="2">
-        <v>448</v>
+        <v>612</v>
       </c>
       <c r="L131" t="s" s="2">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="M131" t="s" s="2">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="N131" t="s" s="2">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="O131" t="s" s="2">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="P131" t="s" s="2">
         <v>82</v>
@@ -18154,7 +18156,7 @@
         <v>82</v>
       </c>
       <c r="AL131" t="s" s="2">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="AM131" t="s" s="2">
         <v>455</v>
@@ -18171,10 +18173,10 @@
     </row>
     <row r="132" hidden="true">
       <c r="A132" t="s" s="2">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="B132" t="s" s="2">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="C132" s="2"/>
       <c r="D132" t="s" s="2">
@@ -18200,13 +18202,13 @@
         <v>198</v>
       </c>
       <c r="L132" t="s" s="2">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="M132" t="s" s="2">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="N132" t="s" s="2">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="O132" t="s" s="2">
         <v>462</v>
@@ -18258,7 +18260,7 @@
         <v>82</v>
       </c>
       <c r="AF132" t="s" s="2">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="AG132" t="s" s="2">
         <v>80</v>
@@ -18293,10 +18295,10 @@
     </row>
     <row r="133" hidden="true">
       <c r="A133" t="s" s="2">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="B133" t="s" s="2">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="C133" s="2"/>
       <c r="D133" t="s" s="2">
@@ -18380,7 +18382,7 @@
         <v>82</v>
       </c>
       <c r="AF133" t="s" s="2">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="AG133" t="s" s="2">
         <v>80</v>
@@ -18415,10 +18417,10 @@
     </row>
     <row r="134" hidden="true">
       <c r="A134" t="s" s="2">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="B134" t="s" s="2">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="C134" s="2"/>
       <c r="D134" t="s" s="2">
@@ -18444,10 +18446,10 @@
         <v>83</v>
       </c>
       <c r="L134" t="s" s="2">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="M134" t="s" s="2">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="N134" t="s" s="2">
         <v>529</v>
@@ -18502,7 +18504,7 @@
         <v>82</v>
       </c>
       <c r="AF134" t="s" s="2">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="AG134" t="s" s="2">
         <v>80</v>

</xml_diff>